<commit_message>
atualizações na tela de professor e coordenador, inserção maanual de aluno e inserção de planilha
</commit_message>
<xml_diff>
--- a/log_acessos.xlsx
+++ b/log_acessos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C98"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -739,6 +739,1366 @@
         </is>
       </c>
     </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>coord123</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>2025-05-24</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>16:55:59</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>profana</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>2025-05-24</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>16:56:19</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>profana</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>2025-05-24</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>14:03:16</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>coord123</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>2025-05-29</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>15:44:59</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>coord123</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>2025-05-29</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>15:58:17</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>coord123</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>2025-05-29</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>16:03:41</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>coord123</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>2025-05-29</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>16:05:50</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>coord123</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>2025-05-29</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>16:06:17</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>coord123</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>2025-05-29</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>16:08:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>coord123</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>2025-05-29</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>16:12:07</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>coord123</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>2025-05-29</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>16:27:33</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>coord123</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>2025-05-29</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>16:29:17</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>coord123</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>2025-05-29</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>16:30:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>coord123</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>2025-05-29</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>16:46:16</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>coord123</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>2025-05-29</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>16:47:24</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>coord123</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>2025-05-29</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>16:49:23</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>coord123</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>2025-05-29</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>16:50:32</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>coord123</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>2025-05-29</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>16:51:50</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>coord123</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>2025-05-29</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>17:31:39</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>coord123</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>2025-05-29</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>17:32:24</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>coord123</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>2025-05-29</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>17:33:11</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>coord123</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>2025-05-29</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>17:37:14</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>coord123</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>2025-05-29</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>17:39:51</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>profana</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>2025-05-29</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>17:48:55</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>profana</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>2025-05-29</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>17:52:13</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>coord123</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>2025-05-29</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>17:52:41</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>profana</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>2025-05-29</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>17:53:07</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>profana</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>2025-05-29</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>17:57:40</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>profana</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>2025-05-29</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>17:58:59</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>profana</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>2025-05-29</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>18:00:20</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>profana</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>2025-05-29</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>18:01:39</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>coord123</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>2025-05-29</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>18:35:01</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>coord123</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>2025-05-29</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>18:39:29</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>coord123</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>2025-05-29</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>18:40:21</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>coord123</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>2025-05-29</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>18:42:47</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>coord123</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>2025-05-29</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>18:45:30</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>coord123</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>2025-05-29</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>18:48:58</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>coord123</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>2025-05-29</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>18:50:26</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>coord123</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>2025-05-29</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>19:03:05</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>profana</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>2025-05-29</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>19:15:40</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>coord123</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>2025-05-29</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>19:31:36</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>coord123</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>2025-05-29</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>19:34:43</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>profana</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>2025-05-29</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>19:37:05</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>profana</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>2025-05-29</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>19:40:55</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>profana</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>2025-05-29</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>19:45:21</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>coord123</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>2025-05-29</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>19:45:55</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>profana</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>2025-05-29</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>19:46:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>coord123</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>2025-05-29</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>19:48:43</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>coord123</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>2025-05-29</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>19:49:53</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>coord123</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>2025-05-29</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>19:52:04</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>coord123</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>2025-05-29</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>19:53:51</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>coord123</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>2025-05-29</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>19:54:48</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>coord123</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>2025-05-29</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>19:56:01</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>coord123</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>2025-05-29</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>19:57:05</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>coord123</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>2025-05-29</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>19:57:13</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>coord123</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>2025-05-29</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>19:58:47</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>coord123</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>2025-05-29</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>20:11:35</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>coord123</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>2025-05-29</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>20:14:18</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>coord123</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>2025-05-29</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>20:14:52</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>coord123</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>2025-05-29</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>20:15:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>profana</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>2025-05-29</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>20:17:50</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>coord123</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>2025-05-29</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>20:17:59</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>coord123</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>2025-05-29</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>20:19:05</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>coord123</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>2025-05-29</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>20:20:15</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>coord123</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>2025-05-29</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>20:22:04</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>coord123</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>2025-05-29</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>20:22:40</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>coord123</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>2025-05-29</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>20:23:17</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>profana</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>2025-05-29</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>20:24:30</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>profana</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>2025-05-29</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>20:24:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>profana</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>2025-05-29</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>20:26:46</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>coord123</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>2025-05-29</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>20:27:12</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>coord123</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>2025-05-29</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>20:28:37</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>coord123</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>2025-05-29</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>20:31:53</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>profana</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>2025-05-29</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>20:32:34</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>coord123</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>2025-05-29</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>20:34:37</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>profana</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>2025-05-29</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>20:35:16</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>coord123</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>2025-05-29</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>20:35:37</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>profana</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>2025-05-29</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>20:35:49</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>coord123</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>2025-05-29</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>20:40:35</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>profana</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>2025-05-29</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>20:41:24</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Adiciona a função de comparar o aluno com a média do curso
</commit_message>
<xml_diff>
--- a/log_acessos.xlsx
+++ b/log_acessos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C98"/>
+  <dimension ref="A1:C100"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2099,6 +2099,40 @@
         </is>
       </c>
     </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>coord123</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>2025-06-03</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>01:38:39</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>coord123</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>2025-06-03</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>02:03:03</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
alteraçoes do estilo e disposiçoes dos elementos na tela, adiçao da funcioanlidade de visualizar por curso e semestre e evoluçao do aluno
</commit_message>
<xml_diff>
--- a/log_acessos.xlsx
+++ b/log_acessos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C100"/>
+  <dimension ref="A1:C132"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2133,6 +2133,550 @@
         </is>
       </c>
     </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>coord123</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>2025-06-04</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>15:28:20</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>coord123</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>2025-06-04</t>
+        </is>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>15:32:02</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>coord123</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>2025-06-04</t>
+        </is>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>15:33:20</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>coord123</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>2025-06-04</t>
+        </is>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>15:34:53</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>profana</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>2025-06-04</t>
+        </is>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>15:37:15</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>coord123</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>2025-06-04</t>
+        </is>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>15:37:50</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>coord123</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>2025-06-04</t>
+        </is>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>15:50:52</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>coord123</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>2025-06-04</t>
+        </is>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>16:01:40</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>coord123</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>2025-06-04</t>
+        </is>
+      </c>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>16:04:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>coord123</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>2025-06-04</t>
+        </is>
+      </c>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t>16:07:05</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>coord123</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>2025-06-04</t>
+        </is>
+      </c>
+      <c r="C111" t="inlineStr">
+        <is>
+          <t>16:07:41</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>profana</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>2025-06-04</t>
+        </is>
+      </c>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t>16:14:56</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>profana</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>2025-06-04</t>
+        </is>
+      </c>
+      <c r="C113" t="inlineStr">
+        <is>
+          <t>16:16:27</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>profana</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>2025-06-04</t>
+        </is>
+      </c>
+      <c r="C114" t="inlineStr">
+        <is>
+          <t>16:17:05</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>profana</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>2025-06-04</t>
+        </is>
+      </c>
+      <c r="C115" t="inlineStr">
+        <is>
+          <t>16:17:55</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>profana</t>
+        </is>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>2025-06-04</t>
+        </is>
+      </c>
+      <c r="C116" t="inlineStr">
+        <is>
+          <t>16:18:03</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>profana</t>
+        </is>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>2025-06-04</t>
+        </is>
+      </c>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>16:18:48</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>profana</t>
+        </is>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>2025-06-04</t>
+        </is>
+      </c>
+      <c r="C118" t="inlineStr">
+        <is>
+          <t>16:31:35</t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>profana</t>
+        </is>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>2025-06-04</t>
+        </is>
+      </c>
+      <c r="C119" t="inlineStr">
+        <is>
+          <t>16:33:09</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>profana</t>
+        </is>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>2025-06-04</t>
+        </is>
+      </c>
+      <c r="C120" t="inlineStr">
+        <is>
+          <t>16:33:37</t>
+        </is>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>profana</t>
+        </is>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>2025-06-04</t>
+        </is>
+      </c>
+      <c r="C121" t="inlineStr">
+        <is>
+          <t>16:41:41</t>
+        </is>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>profana</t>
+        </is>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>2025-06-04</t>
+        </is>
+      </c>
+      <c r="C122" t="inlineStr">
+        <is>
+          <t>16:44:30</t>
+        </is>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>profana</t>
+        </is>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>2025-06-04</t>
+        </is>
+      </c>
+      <c r="C123" t="inlineStr">
+        <is>
+          <t>16:46:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="inlineStr">
+        <is>
+          <t>profana</t>
+        </is>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t>2025-06-04</t>
+        </is>
+      </c>
+      <c r="C124" t="inlineStr">
+        <is>
+          <t>16:51:07</t>
+        </is>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="inlineStr">
+        <is>
+          <t>coord123</t>
+        </is>
+      </c>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>2025-06-04</t>
+        </is>
+      </c>
+      <c r="C125" t="inlineStr">
+        <is>
+          <t>16:52:39</t>
+        </is>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="inlineStr">
+        <is>
+          <t>coord123</t>
+        </is>
+      </c>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>2025-06-04</t>
+        </is>
+      </c>
+      <c r="C126" t="inlineStr">
+        <is>
+          <t>16:53:36</t>
+        </is>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="inlineStr">
+        <is>
+          <t>coord123</t>
+        </is>
+      </c>
+      <c r="B127" t="inlineStr">
+        <is>
+          <t>2025-06-04</t>
+        </is>
+      </c>
+      <c r="C127" t="inlineStr">
+        <is>
+          <t>16:54:32</t>
+        </is>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="inlineStr">
+        <is>
+          <t>coord123</t>
+        </is>
+      </c>
+      <c r="B128" t="inlineStr">
+        <is>
+          <t>2025-06-04</t>
+        </is>
+      </c>
+      <c r="C128" t="inlineStr">
+        <is>
+          <t>16:54:55</t>
+        </is>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="inlineStr">
+        <is>
+          <t>coord123</t>
+        </is>
+      </c>
+      <c r="B129" t="inlineStr">
+        <is>
+          <t>2025-06-04</t>
+        </is>
+      </c>
+      <c r="C129" t="inlineStr">
+        <is>
+          <t>18:45:28</t>
+        </is>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="inlineStr">
+        <is>
+          <t>coord123</t>
+        </is>
+      </c>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t>2025-06-04</t>
+        </is>
+      </c>
+      <c r="C130" t="inlineStr">
+        <is>
+          <t>18:46:05</t>
+        </is>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="inlineStr">
+        <is>
+          <t>profana</t>
+        </is>
+      </c>
+      <c r="B131" t="inlineStr">
+        <is>
+          <t>2025-06-04</t>
+        </is>
+      </c>
+      <c r="C131" t="inlineStr">
+        <is>
+          <t>18:51:30</t>
+        </is>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="inlineStr">
+        <is>
+          <t>coord123</t>
+        </is>
+      </c>
+      <c r="B132" t="inlineStr">
+        <is>
+          <t>2025-06-04</t>
+        </is>
+      </c>
+      <c r="C132" t="inlineStr">
+        <is>
+          <t>18:58:37</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>